<commit_message>
modified script: data_mining_analysis, Results_2018.doc
</commit_message>
<xml_diff>
--- a/Results/sum_table.xlsx
+++ b/Results/sum_table.xlsx
@@ -1,26 +1,117 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\kemushi\Macaca-population-trend\Results\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="20" windowWidth="16100" windowHeight="9660" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Group" sheetId="1" r:id="rId1"/>
     <sheet name="Single" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="27">
+  <si>
+    <t>County</t>
+  </si>
+  <si>
+    <t>dataN_2015</t>
+  </si>
+  <si>
+    <t>dataN_2016</t>
+  </si>
+  <si>
+    <t>dataN_2017</t>
+  </si>
+  <si>
+    <t>dataN_2018</t>
+  </si>
+  <si>
+    <t>SiteN_2015</t>
+  </si>
+  <si>
+    <t>SiteN_2016</t>
+  </si>
+  <si>
+    <t>SiteN_2017</t>
+  </si>
+  <si>
+    <t>SiteN_2018</t>
+  </si>
+  <si>
+    <t>PointN_2015</t>
+  </si>
+  <si>
+    <t>PointN_2016</t>
+  </si>
+  <si>
+    <t>PointN_2017</t>
+  </si>
+  <si>
+    <t>PointN_2018</t>
+  </si>
+  <si>
+    <t>南投縣</t>
+  </si>
+  <si>
+    <t>台中市</t>
+  </si>
+  <si>
+    <t>台北市</t>
+  </si>
+  <si>
+    <t>台南市</t>
+  </si>
+  <si>
+    <t>台東縣</t>
+  </si>
+  <si>
+    <t>嘉義縣</t>
+  </si>
+  <si>
+    <t>宜蘭縣</t>
+  </si>
+  <si>
+    <t>屏東縣</t>
+  </si>
+  <si>
+    <t>新北市</t>
+  </si>
+  <si>
+    <t>花蓮縣</t>
+  </si>
+  <si>
+    <t>苗栗縣</t>
+  </si>
+  <si>
+    <t>雲林縣</t>
+  </si>
+  <si>
+    <t>高雄市</t>
+  </si>
+  <si>
+    <t>嘉義市</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -28,8 +119,15 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="新細明體"/>
+      <family val="3"/>
+      <charset val="136"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -60,15 +158,23 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -110,7 +216,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -142,9 +248,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -176,6 +283,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -351,85 +459,59 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15:M15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>County</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>dataN_2015</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>dataN_2016</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>dataN_2017</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>dataN_2018</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>SiteN_2015</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>SiteN_2016</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>SiteN_2017</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>SiteN_2018</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>PointN_2015</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>PointN_2016</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>PointN_2017</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>PointN_2018</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>南投縣</t>
-        </is>
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>13</v>
       </c>
       <c r="B2">
         <v>7</v>
@@ -468,11 +550,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>台中市</t>
-        </is>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>14</v>
       </c>
       <c r="B3">
         <v>8</v>
@@ -511,11 +591,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>台北市</t>
-        </is>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>15</v>
       </c>
       <c r="D4">
         <v>3</v>
@@ -536,11 +614,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>台南市</t>
-        </is>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>16</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -570,11 +646,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>台東縣</t>
-        </is>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>17</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -613,11 +687,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>嘉義縣</t>
-        </is>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>18</v>
       </c>
       <c r="B7">
         <v>5</v>
@@ -656,11 +728,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>宜蘭縣</t>
-        </is>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>19</v>
       </c>
       <c r="B8">
         <v>6</v>
@@ -690,11 +760,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>屏東縣</t>
-        </is>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>20</v>
       </c>
       <c r="B9">
         <v>3</v>
@@ -733,11 +801,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>新北市</t>
-        </is>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>21</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -767,11 +833,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>花蓮縣</t>
-        </is>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>22</v>
       </c>
       <c r="B11">
         <v>16</v>
@@ -810,11 +874,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>苗栗縣</t>
-        </is>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>23</v>
       </c>
       <c r="B12">
         <v>3</v>
@@ -844,11 +906,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>雲林縣</t>
-        </is>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>24</v>
       </c>
       <c r="B13">
         <v>9</v>
@@ -887,11 +947,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>高雄市</t>
-        </is>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>25</v>
       </c>
       <c r="B14">
         <v>7</v>
@@ -930,91 +988,117 @@
         <v>6</v>
       </c>
     </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B15">
+        <f>SUM(B2:B14)</f>
+        <v>68</v>
+      </c>
+      <c r="C15">
+        <f t="shared" ref="C15:M15" si="0">SUM(C2:C14)</f>
+        <v>47</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="0"/>
+        <v>72</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>County</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>dataN_2015</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>dataN_2016</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>dataN_2017</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>dataN_2018</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>SiteN_2015</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>SiteN_2016</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>SiteN_2017</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>SiteN_2018</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>PointN_2015</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>PointN_2016</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>PointN_2017</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>PointN_2018</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>南投縣</t>
-        </is>
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>13</v>
       </c>
       <c r="B2">
         <v>2</v>
@@ -1053,11 +1137,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>台中市</t>
-        </is>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>14</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -1096,11 +1178,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>台北市</t>
-        </is>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>15</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -1112,11 +1192,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>台東縣</t>
-        </is>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>17</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1137,11 +1215,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>嘉義市</t>
-        </is>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>26</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -1153,11 +1229,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>嘉義縣</t>
-        </is>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>18</v>
       </c>
       <c r="B7">
         <v>3</v>
@@ -1178,11 +1252,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>宜蘭縣</t>
-        </is>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>19</v>
       </c>
       <c r="C8">
         <v>3</v>
@@ -1194,11 +1266,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>屏東縣</t>
-        </is>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>20</v>
       </c>
       <c r="C9">
         <v>3</v>
@@ -1228,11 +1298,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>新北市</t>
-        </is>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>21</v>
       </c>
       <c r="B10">
         <v>2</v>
@@ -1244,11 +1312,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>花蓮縣</t>
-        </is>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>22</v>
       </c>
       <c r="B11">
         <v>8</v>
@@ -1287,11 +1353,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>苗栗縣</t>
-        </is>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>23</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -1303,11 +1367,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>雲林縣</t>
-        </is>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>24</v>
       </c>
       <c r="B13">
         <v>4</v>
@@ -1337,11 +1399,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>高雄市</t>
-        </is>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>25</v>
       </c>
       <c r="B14">
         <v>7</v>
@@ -1380,7 +1440,58 @@
         <v>1</v>
       </c>
     </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B15">
+        <f>SUM(B2:B14)</f>
+        <v>31</v>
+      </c>
+      <c r="C15">
+        <f t="shared" ref="C15:M15" si="0">SUM(C2:C14)</f>
+        <v>19</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>